<commit_message>
redo with new data where NTCs passed
</commit_message>
<xml_diff>
--- a/TN052.13/filtered_results.xlsx
+++ b/TN052.13/filtered_results.xlsx
@@ -472,7 +472,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>4.8661995</v>
+        <v>4.570121</v>
       </c>
     </row>
     <row r="3">
@@ -492,7 +492,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.8762593</v>
+        <v>4.429555</v>
       </c>
     </row>
     <row r="4">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.90172</v>
+        <v>4.3924713</v>
       </c>
     </row>
     <row r="5">
@@ -532,7 +532,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5.021006</v>
+        <v>4.475478</v>
       </c>
     </row>
     <row r="6">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.990601</v>
+        <v>4.8108716</v>
       </c>
     </row>
     <row r="7">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.9730597</v>
+        <v>4.62121</v>
       </c>
     </row>
     <row r="8">
@@ -592,7 +592,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4.855776</v>
+        <v>4.427797</v>
       </c>
     </row>
     <row r="9">
@@ -612,7 +612,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>4.8342357</v>
+        <v>4.4477773</v>
       </c>
     </row>
     <row r="10">
@@ -632,7 +632,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>4.83664</v>
+        <v>4.4033685</v>
       </c>
     </row>
     <row r="11">
@@ -652,7 +652,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>20.087545</v>
+        <v>20.044765</v>
       </c>
     </row>
     <row r="12">
@@ -672,7 +672,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>20.045673</v>
+        <v>20.09938</v>
       </c>
     </row>
     <row r="13">
@@ -692,7 +692,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>20.085316</v>
+        <v>20.093447</v>
       </c>
     </row>
     <row r="14">
@@ -712,7 +712,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>19.913982</v>
+        <v>19.954018</v>
       </c>
     </row>
     <row r="15">
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>19.975006</v>
+        <v>20.11724</v>
       </c>
     </row>
     <row r="16">
@@ -752,7 +752,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>20.063023</v>
+        <v>20.191637</v>
       </c>
     </row>
     <row r="17">
@@ -772,7 +772,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>19.80701</v>
+        <v>19.834846</v>
       </c>
     </row>
     <row r="18">
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>19.808168</v>
+        <v>19.86631</v>
       </c>
     </row>
     <row r="19">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>19.782085</v>
+        <v>19.858034</v>
       </c>
     </row>
     <row r="20">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>5.8274393</v>
+        <v>5.340901</v>
       </c>
     </row>
     <row r="21">
@@ -852,7 +852,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>5.763424</v>
+        <v>5.433157</v>
       </c>
     </row>
     <row r="22">
@@ -872,7 +872,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>5.752831</v>
+        <v>5.1576967</v>
       </c>
     </row>
     <row r="23">
@@ -892,7 +892,7 @@
         </is>
       </c>
       <c r="D23" t="n">
-        <v>5.0148025</v>
+        <v>4.4378176</v>
       </c>
     </row>
     <row r="24">
@@ -912,7 +912,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>4.9322658</v>
+        <v>4.4187546</v>
       </c>
     </row>
     <row r="25">
@@ -932,7 +932,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>4.947193</v>
+        <v>4.51871</v>
       </c>
     </row>
     <row r="26">
@@ -952,7 +952,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>4.716456</v>
+        <v>4.3101935</v>
       </c>
     </row>
     <row r="27">
@@ -972,7 +972,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>4.880707</v>
+        <v>4.423321</v>
       </c>
     </row>
     <row r="28">
@@ -992,7 +992,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>4.923984</v>
+        <v>4.4769</v>
       </c>
     </row>
     <row r="29">
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>21.02475</v>
+        <v>21.09741</v>
       </c>
     </row>
     <row r="30">
@@ -1032,7 +1032,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>21.00204</v>
+        <v>20.952942</v>
       </c>
     </row>
     <row r="31">
@@ -1052,7 +1052,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>21.16563</v>
+        <v>20.861547</v>
       </c>
     </row>
     <row r="32">
@@ -1072,7 +1072,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>20.238491</v>
+        <v>20.21614</v>
       </c>
     </row>
     <row r="33">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>20.146255</v>
+        <v>20.162424</v>
       </c>
     </row>
     <row r="34">
@@ -1112,7 +1112,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>20.23893</v>
+        <v>20.3171</v>
       </c>
     </row>
     <row r="35">
@@ -1132,7 +1132,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>19.682348</v>
+        <v>19.750463</v>
       </c>
     </row>
     <row r="36">
@@ -1152,7 +1152,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>19.875593</v>
+        <v>19.930487</v>
       </c>
     </row>
     <row r="37">
@@ -1172,7 +1172,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>19.950155</v>
+        <v>19.97378</v>
       </c>
     </row>
     <row r="38">
@@ -1192,7 +1192,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>5.0330296</v>
+        <v>4.8195386</v>
       </c>
     </row>
     <row r="39">
@@ -1212,7 +1212,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>5.096067</v>
+        <v>4.5988398</v>
       </c>
     </row>
     <row r="40">
@@ -1232,7 +1232,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>5.066455</v>
+        <v>4.704048</v>
       </c>
     </row>
     <row r="41">
@@ -1252,7 +1252,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>4.949909</v>
+        <v>4.4755135</v>
       </c>
     </row>
     <row r="42">
@@ -1272,7 +1272,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>4.960425</v>
+        <v>4.471478</v>
       </c>
     </row>
     <row r="43">
@@ -1292,7 +1292,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>4.8226295</v>
+        <v>4.465045</v>
       </c>
     </row>
     <row r="44">
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>4.9807134</v>
+        <v>4.449566</v>
       </c>
     </row>
     <row r="45">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>4.8097577</v>
+        <v>4.3526654</v>
       </c>
     </row>
     <row r="46">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="D46" t="n">
-        <v>4.9011755</v>
+        <v>4.479339</v>
       </c>
     </row>
     <row r="47">
@@ -1372,7 +1372,7 @@
         </is>
       </c>
       <c r="D47" t="n">
-        <v>20.1162</v>
+        <v>20.194372</v>
       </c>
     </row>
     <row r="48">
@@ -1392,7 +1392,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>20.137386</v>
+        <v>20.077696</v>
       </c>
     </row>
     <row r="49">
@@ -1412,7 +1412,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>20.065338</v>
+        <v>20.025795</v>
       </c>
     </row>
     <row r="50">
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>19.9725</v>
+        <v>20.066381</v>
       </c>
     </row>
     <row r="51">
@@ -1452,7 +1452,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>19.984695</v>
+        <v>19.973536</v>
       </c>
     </row>
     <row r="52">
@@ -1472,7 +1472,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>19.988811</v>
+        <v>20.033766</v>
       </c>
     </row>
     <row r="53">
@@ -1492,7 +1492,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>19.947763</v>
+        <v>19.903559</v>
       </c>
     </row>
     <row r="54">
@@ -1512,7 +1512,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>19.887512</v>
+        <v>19.973228</v>
       </c>
     </row>
     <row r="55">
@@ -1532,7 +1532,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>19.788113</v>
+        <v>19.778542</v>
       </c>
     </row>
     <row r="56">
@@ -1552,7 +1552,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>5.016702</v>
+        <v>4.989229</v>
       </c>
     </row>
     <row r="57">
@@ -1572,7 +1572,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>4.9764824</v>
+        <v>4.570296</v>
       </c>
     </row>
     <row r="58">
@@ -1592,7 +1592,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>4.9192514</v>
+        <v>4.520977</v>
       </c>
     </row>
     <row r="59">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>4.8780336</v>
+        <v>4.466665</v>
       </c>
     </row>
     <row r="60">
@@ -1632,7 +1632,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>4.8686543</v>
+        <v>4.3805895</v>
       </c>
     </row>
     <row r="61">
@@ -1652,7 +1652,7 @@
         </is>
       </c>
       <c r="D61" t="n">
-        <v>4.8514414</v>
+        <v>4.465386</v>
       </c>
     </row>
     <row r="62">
@@ -1672,7 +1672,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>4.873271</v>
+        <v>4.540096</v>
       </c>
     </row>
     <row r="63">
@@ -1692,7 +1692,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>4.8324404</v>
+        <v>4.4209065</v>
       </c>
     </row>
     <row r="64">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>4.8481264</v>
+        <v>4.407012</v>
       </c>
     </row>
     <row r="65">
@@ -1732,7 +1732,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>20.054008</v>
+        <v>20.196901</v>
       </c>
     </row>
     <row r="66">
@@ -1752,7 +1752,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>20.099188</v>
+        <v>20.066807</v>
       </c>
     </row>
     <row r="67">
@@ -1772,7 +1772,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>20.04346</v>
+        <v>20.043415</v>
       </c>
     </row>
     <row r="68">
@@ -1792,7 +1792,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>19.968145</v>
+        <v>19.957195</v>
       </c>
     </row>
     <row r="69">
@@ -1812,7 +1812,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>19.942554</v>
+        <v>19.960686</v>
       </c>
     </row>
     <row r="70">
@@ -1832,7 +1832,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>19.888557</v>
+        <v>19.969162</v>
       </c>
     </row>
     <row r="71">
@@ -1852,7 +1852,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>20.126972</v>
+        <v>20.160696</v>
       </c>
     </row>
     <row r="72">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>20.06536</v>
+        <v>20.111479</v>
       </c>
     </row>
     <row r="73">
@@ -1892,7 +1892,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>20.09608</v>
+        <v>20.14878</v>
       </c>
     </row>
   </sheetData>

</xml_diff>